<commit_message>
Add DP pickups Working on Android distribution Iterating on GUI for Save/Load, store
</commit_message>
<xml_diff>
--- a/Source/ProjectHunt/Resources/DataTables/Weapons/PistolUpgradeTable.xlsx
+++ b/Source/ProjectHunt/Resources/DataTables/Weapons/PistolUpgradeTable.xlsx
@@ -1,55 +1,68 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Etern\Unreal Projects\ProjectHunt\Source\ProjectHunt\Resources\DataTables\Weapons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DA7CA5-E3DC-4D84-B7BA-DC5C1176D4C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7016FF55-484C-4502-B64E-779D60FB0D62}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PistolUpgradeTable" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>NewWeaponLevel</t>
+    <t>WeaponDamageLevel</t>
   </si>
   <si>
     <t>DamageUpgradeAmount</t>
   </si>
   <si>
+    <t>DamageUpgradePrice</t>
+  </si>
+  <si>
+    <t>FireRateLevel</t>
+  </si>
+  <si>
     <t>FireRateUpgradeAmount</t>
+  </si>
+  <si>
+    <t>FireRateUpgradePrice</t>
+  </si>
+  <si>
+    <t>ChargeRateLevel</t>
   </si>
   <si>
     <t>ChargeRateAmountIncrease</t>
   </si>
   <si>
+    <t>ChargeLimitLevel</t>
+  </si>
+  <si>
     <t>ChargeLimitAmountIncrease</t>
   </si>
   <si>
-    <t>WeaponUpgradePrice</t>
+    <t>ChargeLimitUpgradePrice</t>
+  </si>
+  <si>
+    <t>ChargeRateUpgradePrice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,16 +70,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -74,15 +387,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -114,7 +616,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -126,7 +628,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -173,6 +675,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -208,6 +727,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -360,23 +896,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -395,8 +938,26 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -407,16 +968,37 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2">
+        <v>1000</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>0.02</v>
+      </c>
+      <c r="J2">
+        <v>1000</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>0.02</v>
+      </c>
+      <c r="M2">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -427,10 +1009,10 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -438,8 +1020,26 @@
       <c r="G3">
         <v>2000</v>
       </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>0.02</v>
+      </c>
+      <c r="J3">
+        <v>2000</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>0.05</v>
+      </c>
+      <c r="M3">
+        <v>2000</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -450,19 +1050,37 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="E4">
-        <v>0.02</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>3000</v>
       </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>0.02</v>
+      </c>
+      <c r="J4">
+        <v>3000</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>0.05</v>
+      </c>
+      <c r="M4">
+        <v>3000</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -473,19 +1091,37 @@
         <v>3.5</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="E5">
-        <v>0.02</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>4000</v>
       </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>0.02</v>
+      </c>
+      <c r="J5">
+        <v>4000</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>0.02</v>
+      </c>
+      <c r="M5">
+        <v>4000</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -496,19 +1132,37 @@
         <v>0.5</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="E6">
-        <v>0.02</v>
+        <v>6</v>
       </c>
       <c r="F6">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>5000</v>
       </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>0.02</v>
+      </c>
+      <c r="J6">
+        <v>5000</v>
+      </c>
+      <c r="K6">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <v>0.02</v>
+      </c>
+      <c r="M6">
+        <v>5000</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -519,19 +1173,37 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>3000</v>
       </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>3000</v>
+      </c>
+      <c r="K7">
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <v>0.02</v>
+      </c>
+      <c r="M7">
+        <v>3000</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -542,10 +1214,10 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -553,8 +1225,26 @@
       <c r="G8">
         <v>4000</v>
       </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>4000</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>4000</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -565,10 +1255,10 @@
         <v>3</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -576,8 +1266,26 @@
       <c r="G9">
         <v>5000</v>
       </c>
+      <c r="H9">
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>5000</v>
+      </c>
+      <c r="K9">
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>5000</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -588,19 +1296,37 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="E10">
-        <v>0.02</v>
+        <v>10</v>
       </c>
       <c r="F10">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>6000</v>
       </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>0.02</v>
+      </c>
+      <c r="J10">
+        <v>6000</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>0.02</v>
+      </c>
+      <c r="M10">
+        <v>6000</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -611,20 +1337,37 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>7000</v>
       </c>
       <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>7000</v>
+      </c>
+      <c r="H11">
+        <v>11</v>
+      </c>
+      <c r="I11">
         <v>0.02</v>
       </c>
-      <c r="F11">
+      <c r="J11">
+        <v>7000</v>
+      </c>
+      <c r="K11">
+        <v>11</v>
+      </c>
+      <c r="L11">
         <v>0.02</v>
       </c>
-      <c r="G11">
+      <c r="M11">
         <v>7000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>